<commit_message>
Fix a bug. Make rat avoid walls. Update a graphical performance
</commit_message>
<xml_diff>
--- a/Lab1/Statistcs.xlsx
+++ b/Lab1/Statistcs.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/xisung/Desktop/StudyHard/AlgorithmandDiscretMath/AI_XiS/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/xisung/Desktop/StudyHard/AlgorithmandDiscretMath/AI_XiS/Lab1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D9FCF24-584B-EC4F-9043-1BECC1FC2A8A}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EC8BAC3-CCC3-2241-993E-1B1F620A0028}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000" xr2:uid="{AC0F846C-F511-324A-AA18-2684E59D13D5}"/>
+    <workbookView xWindow="20140" yWindow="5320" windowWidth="15720" windowHeight="14460" xr2:uid="{AC0F846C-F511-324A-AA18-2684E59D13D5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="20">
   <si>
     <t>default</t>
   </si>
@@ -48,58 +48,43 @@
     <t>Density of Wall and Mud</t>
   </si>
   <si>
-    <t>34/68/114</t>
-  </si>
-  <si>
-    <t>40/82/158</t>
-  </si>
-  <si>
-    <t>4/23/36</t>
-  </si>
-  <si>
-    <t>656/26/398</t>
-  </si>
-  <si>
-    <t>748/28/417</t>
-  </si>
-  <si>
-    <t>173/0/212</t>
-  </si>
-  <si>
-    <t>66/232/92</t>
-  </si>
-  <si>
-    <t>88/259/121</t>
-  </si>
-  <si>
-    <t>15/132/51</t>
-  </si>
-  <si>
-    <t>38/14/16</t>
-  </si>
-  <si>
-    <t>40/43/21</t>
-  </si>
-  <si>
-    <t>10/4/19</t>
-  </si>
-  <si>
-    <t>32/36/10</t>
-  </si>
-  <si>
-    <t>49/46/10</t>
-  </si>
-  <si>
-    <t>46/0/17</t>
-  </si>
-  <si>
-    <t>4/4/4</t>
-  </si>
-  <si>
-    <t>7/4/4</t>
-  </si>
-  <si>
-    <t>0/0/4</t>
+    <t>0/0/0</t>
+  </si>
+  <si>
+    <t>58/802/60</t>
+  </si>
+  <si>
+    <t>38/233/22</t>
+  </si>
+  <si>
+    <t>184/100/14</t>
+  </si>
+  <si>
+    <t>99/114/4</t>
+  </si>
+  <si>
+    <t>94/318/66</t>
+  </si>
+  <si>
+    <t>31/246/12</t>
+  </si>
+  <si>
+    <t>32/40/46</t>
+  </si>
+  <si>
+    <t>12/33/21</t>
+  </si>
+  <si>
+    <t>24/10/12</t>
+  </si>
+  <si>
+    <t>14/0/0</t>
+  </si>
+  <si>
+    <t>2/4/4</t>
+  </si>
+  <si>
+    <t>0/0/2</t>
   </si>
 </sst>
 </file>
@@ -467,8 +452,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{153C3645-FDB3-1241-9D47-B17E26252A83}">
   <dimension ref="A1:F7"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="187" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="187" workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -476,7 +461,9 @@
     <col min="1" max="1" width="31.6640625" style="2" customWidth="1"/>
     <col min="2" max="2" width="16" style="2" customWidth="1"/>
     <col min="3" max="3" width="15.6640625" style="2" customWidth="1"/>
-    <col min="4" max="16384" width="10.83203125" style="2"/>
+    <col min="4" max="4" width="14.6640625" style="2" customWidth="1"/>
+    <col min="5" max="6" width="16.33203125" style="2" customWidth="1"/>
+    <col min="7" max="16384" width="10.83203125" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -510,13 +497,13 @@
         <v>3</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>23</v>
+        <v>7</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
@@ -530,13 +517,13 @@
         <v>5</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>20</v>
+        <v>7</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
@@ -550,13 +537,13 @@
         <v>7</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
@@ -570,13 +557,13 @@
         <v>9</v>
       </c>
       <c r="D5" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F5" s="2" t="s">
         <v>13</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
@@ -590,13 +577,13 @@
         <v>11</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
@@ -610,13 +597,13 @@
         <v>13</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>